<commit_message>
everything is working now with Lfold!  And the assumptions are all clear and come from the derivation
</commit_message>
<xml_diff>
--- a/parameters/Task15_Param_Ranges_AFIR_Tfold.xlsx
+++ b/parameters/Task15_Param_Ranges_AFIR_Tfold.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256FF231-C494-5546-8DC7-99D3DF375CA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F225CEBF-8DC1-9A4E-9B86-D2FB30805324}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41500" yWindow="460" windowWidth="27300" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task05_Param_Summary" sheetId="1" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>0.0001-1</t>
   </si>
   <si>
-    <t>Tfold</t>
-  </si>
-  <si>
     <t>reasonable ranges (AFIR paper)</t>
   </si>
   <si>
@@ -228,13 +225,16 @@
     <t>type_mem</t>
   </si>
   <si>
-    <t>Lfold</t>
-  </si>
-  <si>
     <t>Conversion: nmol2mpk</t>
   </si>
   <si>
     <t>Kd_DT + keDT/kon_DT</t>
+  </si>
+  <si>
+    <t>keT_keDT_ratio</t>
+  </si>
+  <si>
+    <t>keL_keTL_ratio</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1304,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="163" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1330,22 +1330,22 @@
         <v>29</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>15</v>
@@ -1802,7 +1802,7 @@
         <v>36</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M14" s="1">
         <f>1/mpk2nmol</f>
@@ -1843,7 +1843,7 @@
         <v>34</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1915,7 +1915,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1924,7 +1924,7 @@
         <v>15.5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D18" s="18">
         <f>D19/E20</f>
@@ -1950,7 +1950,7 @@
         <v>46</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -2066,7 +2066,7 @@
         <v>17.5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D22" s="7">
         <v>0.1</v>
@@ -2093,7 +2093,7 @@
         <v>46</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -2356,7 +2356,7 @@
         <v>17</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>